<commit_message>
continue work on paper
</commit_message>
<xml_diff>
--- a/documents/Лист Microsoft Excel.xlsx
+++ b/documents/Лист Microsoft Excel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Artem\Documents\Projects\emotions_aggressive\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CE7D97-5FAE-49B4-812F-652929A36D06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="910" yWindow="-110" windowWidth="18400" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,121 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Год </t>
+  </si>
+  <si>
+    <t>Язык</t>
+  </si>
+  <si>
+    <t>Тип произносимого</t>
+  </si>
+  <si>
+    <t>Дикторы</t>
+  </si>
+  <si>
+    <t>Формат аудио</t>
+  </si>
+  <si>
+    <t>CREMA-D</t>
+  </si>
+  <si>
+    <t>Англ.</t>
+  </si>
+  <si>
+    <t>12 коротких предложений</t>
+  </si>
+  <si>
+    <t>N записей</t>
+  </si>
+  <si>
+    <t>ANG, HAP, SAD, NEU, DIS, FEA</t>
+  </si>
+  <si>
+    <t>IEMOCAP</t>
+  </si>
+  <si>
+    <t>5 мужчин и 5 женщин</t>
+  </si>
+  <si>
+    <t>Диалоги по сценарию и спонтанные импровизации</t>
+  </si>
+  <si>
+    <t>ANG, HAP, SAD, NEU, EXC, FRU</t>
+  </si>
+  <si>
+    <t>Emo-DB</t>
+  </si>
+  <si>
+    <t>Нем.</t>
+  </si>
+  <si>
+    <t>5 коротких и 5 длинных предложений</t>
+  </si>
+  <si>
+    <t>wav, 48 кГц,  2 канала</t>
+  </si>
+  <si>
+    <t>ANG, HAP, SAD, NEU, DIS, FEA, BOR</t>
+  </si>
+  <si>
+    <t>Базовая дискретная разметка</t>
+  </si>
+  <si>
+    <t>RAVDESS</t>
+  </si>
+  <si>
+    <t>ANG, HAP, SAD, NEU, DIS, FEA, SUR, CAL</t>
+  </si>
+  <si>
+    <t>12 мужчин и 12 женщин, от 21 до 33 лет, средний возраст - 26 лет</t>
+  </si>
+  <si>
+    <t>48 мужчин и 43 женщины, возраст от 20 до 74 лет, средний возраст - 36лет</t>
+  </si>
+  <si>
+    <t>2 коротких предложения</t>
+  </si>
+  <si>
+    <t>wav, 48кГц, 2 канала</t>
+  </si>
+  <si>
+    <t>wav, 16кГц, 1 канал</t>
+  </si>
+  <si>
+    <t>4 мужчины, от 27 до 31 года</t>
+  </si>
+  <si>
+    <t xml:space="preserve">120 предложений </t>
+  </si>
+  <si>
+    <t>wav, 44.1кГц, 2 канала</t>
+  </si>
+  <si>
+    <t>ANG, HAP, SAD, NEU, DIS, FEA, SUR</t>
+  </si>
+  <si>
+    <t>SAVEE</t>
+  </si>
+  <si>
+    <t>TESS</t>
+  </si>
+  <si>
+    <t>Фраза 'Say the word X', где Х - одно из 200 односложных слов</t>
+  </si>
+  <si>
+    <t>2 женщины возрастом 26 и 64 года</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,15 +148,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,15 +170,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +479,208 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="G8:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="12.08984375" customWidth="1"/>
+    <col min="8" max="8" width="5.453125" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" customWidth="1"/>
+    <col min="11" max="11" width="29.6328125" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" customWidth="1"/>
+    <col min="13" max="13" width="20.1796875" customWidth="1"/>
+    <col min="14" max="14" width="27.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="7:14" x14ac:dyDescent="0.35">
+      <c r="G8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="7:14" ht="58" x14ac:dyDescent="0.35">
+      <c r="G9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1">
+        <v>2014</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="1">
+        <v>7442</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="7:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="G10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1">
+        <v>2007</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="1">
+        <v>7304</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="7:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2005</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="1">
+        <v>535</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="7:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1">
+        <v>2018</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1440</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="7:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="G13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="1">
+        <v>2008</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="1">
+        <v>480</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="7:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="G14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2020</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="1">
+        <v>2800</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>